<commit_message>
- DS hoadon- chitet: sai công thức sumproduct
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_ChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon_ChiTiet.xlsx
@@ -209,6 +209,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -217,36 +247,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,7 +557,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,24 +567,24 @@
     <col min="3" max="3" width="17.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="21" style="10" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="23" customWidth="1"/>
-    <col min="7" max="8" width="13" style="23" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="16" customWidth="1"/>
+    <col min="7" max="8" width="13" style="16" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="16" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="3" spans="1:9" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -602,16 +602,16 @@
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -621,10 +621,10 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -632,10 +632,10 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -643,10 +643,10 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -654,10 +654,10 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -665,10 +665,10 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -676,10 +676,10 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -687,10 +687,10 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -698,10 +698,10 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -709,10 +709,10 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -720,10 +720,10 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -731,10 +731,10 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -742,10 +742,10 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -753,10 +753,10 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -764,10 +764,10 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -775,10 +775,10 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -786,10 +786,10 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -797,10 +797,10 @@
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -808,10 +808,10 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -819,10 +819,10 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -830,10 +830,10 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -841,10 +841,10 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -852,10 +852,10 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -863,10 +863,10 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -874,99 +874,99 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="22">
-        <f>SUM($E$4:E27)</f>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="15">
+        <f>SUM(E$4:E27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="22">
-        <f>SUMPRODUCT(E4:E27,F4:F27)</f>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="15">
+        <f>SUMPRODUCT(E$4:E27,F$4:F27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="22">
-        <f>SUMPRODUCT(E4:E27,G4:G27)</f>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="15">
+        <f>SUMPRODUCT(E$4:E27,G$4:G27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="22">
-        <f xml:space="preserve"> SUMPRODUCT(E4:E27,H4:H27)</f>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="15">
+        <f xml:space="preserve"> SUMPRODUCT(E$4:E27,H$4:H27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="22">
-        <f>SUM($I$4:I27)</f>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="15">
+        <f>SUM(I$4:I27)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A32:H32"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="A30:H30"/>
     <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.47" bottom="0.45" header="0.3" footer="0.3"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>